<commit_message>
fix empty term in materials vocab
</commit_message>
<xml_diff>
--- a/vocabularies/materials/1.3/materials_1-3.xlsx
+++ b/vocabularies/materials/1.3/materials_1-3.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2000">
   <si>
     <t>synonyms</t>
   </si>
@@ -3524,10 +3524,13 @@
     <t>https://www.mindat.org/min-4410.html</t>
   </si>
   <si>
-    <t>#carbonate minerals#carbonates#carbonate sedimentary rock#carbonate rock#carbonitic rock#carbonate fault#carbonate faults</t>
-  </si>
-  <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-</t>
+    <t>carbonate minerals</t>
+  </si>
+  <si>
+    <t>#carbonates#carbonate sedimentary rock#carbonate rock#carbonitic rock#carbonate fault#carbonate faults</t>
+  </si>
+  <si>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals</t>
   </si>
   <si>
     <t>https://www.mindat.org/strunz.php?a=5</t>
@@ -3536,7 +3539,7 @@
     <t>ankerite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--ankerite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-ankerite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-239.html</t>
@@ -3545,7 +3548,7 @@
     <t>apatite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--apatite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-apatite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-29229.html</t>
@@ -3554,7 +3557,7 @@
     <t>aragonite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--aragonite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-aragonite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-307.html</t>
@@ -3563,7 +3566,7 @@
     <t>azurite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--azurite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-azurite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-447.html</t>
@@ -3572,7 +3575,7 @@
     <t>bastnaesite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--bastnaesite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-bastnaesite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-563.html</t>
@@ -3581,7 +3584,7 @@
     <t>breunnerite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--breunnerite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-breunnerite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-7873.html</t>
@@ -3590,13 +3593,13 @@
     <t>calcite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--calcite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-calcite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-859.html</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--dolomite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-dolomite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-1304.html</t>
@@ -3605,7 +3608,7 @@
     <t>magnesite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--magnesite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-magnesite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-2482.html</t>
@@ -3614,7 +3617,7 @@
     <t>malachite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--malachite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-malachite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-2550.html</t>
@@ -3623,7 +3626,7 @@
     <t>manganocalcite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--manganocalcite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-manganocalcite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-2526.html</t>
@@ -3632,7 +3635,7 @@
     <t>parisite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--parisite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-parisite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-7403.html</t>
@@ -3641,7 +3644,7 @@
     <t>rhodochrosite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--rhodochrosite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-rhodochrosite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-3406.html</t>
@@ -3650,7 +3653,7 @@
     <t>siderite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--siderite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-siderite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-3647.html</t>
@@ -3659,7 +3662,7 @@
     <t>smithsonite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--smithsonite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-smithsonite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-3688.html</t>
@@ -3668,7 +3671,7 @@
     <t>strontianite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--strontianite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-strontianite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-3805.html</t>
@@ -3677,7 +3680,7 @@
     <t>trona</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--trona</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-trona</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-4031.html</t>
@@ -3686,7 +3689,7 @@
     <t>witherite</t>
   </si>
   <si>
-    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals--witherite</t>
+    <t>https://epos-msl.uu.nl/voc/materials/1.3/minerals-carbonate_minerals-witherite</t>
   </si>
   <si>
     <t>https://www.mindat.org/min-4299.html</t>
@@ -6039,15 +6042,19 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10687,91 +10694,94 @@
       </c>
     </row>
     <row r="386" spans="1:9">
+      <c r="B386" t="s">
+        <v>1169</v>
+      </c>
       <c r="F386" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="G386" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="H386" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="387" spans="1:9">
       <c r="C387" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="G387" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="H387" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="388" spans="1:9">
       <c r="C388" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="G388" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="H388" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="389" spans="1:9">
       <c r="C389" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G389" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="H389" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="390" spans="1:9">
       <c r="C390" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="G390" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="H390" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="391" spans="1:9">
       <c r="C391" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="G391" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="H391" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="392" spans="1:9">
       <c r="C392" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="G392" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="H392" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="393" spans="1:9">
       <c r="C393" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="G393" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="H393" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="394" spans="1:9">
@@ -10779,2035 +10789,2035 @@
         <v>67</v>
       </c>
       <c r="G394" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="H394" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="395" spans="1:9">
       <c r="C395" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="G395" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="H395" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="396" spans="1:9">
       <c r="C396" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="G396" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="H396" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="397" spans="1:9">
       <c r="C397" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="G397" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="H397" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="398" spans="1:9">
       <c r="C398" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="G398" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="H398" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="399" spans="1:9">
       <c r="C399" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="G399" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="H399" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="400" spans="1:9">
       <c r="C400" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="G400" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="H400" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="401" spans="1:9">
       <c r="C401" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="G401" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="H401" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="402" spans="1:9">
       <c r="C402" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="G402" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="H402" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="403" spans="1:9">
       <c r="C403" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="G403" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="H403" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="404" spans="1:9">
       <c r="C404" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="G404" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="H404" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="405" spans="1:9">
       <c r="B405" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="G405" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="H405" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="406" spans="1:9">
       <c r="B406" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="G406" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="H406" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="407" spans="1:9">
       <c r="C407" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="G407" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="H407" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="408" spans="1:9">
       <c r="C408" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="G408" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="H408" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="409" spans="1:9">
       <c r="C409" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="G409" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="H409" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="410" spans="1:9">
       <c r="C410" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="G410" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="H410" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="411" spans="1:9">
       <c r="C411" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="G411" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="H411" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="412" spans="1:9">
       <c r="C412" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="G412" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="H412" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="413" spans="1:9">
       <c r="C413" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="G413" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="H413" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="414" spans="1:9">
       <c r="C414" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="G414" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="H414" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="415" spans="1:9">
       <c r="C415" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="G415" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="H415" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="416" spans="1:9">
       <c r="B416" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="G416" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="H416" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="417" spans="1:9">
       <c r="C417" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="G417" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="H417" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="418" spans="1:9">
       <c r="C418" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="G418" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="H418" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="419" spans="1:9">
       <c r="C419" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="G419" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="H419" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="420" spans="1:9">
       <c r="C420" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="G420" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="H420" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="421" spans="1:9">
       <c r="C421" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="G421" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="H421" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="422" spans="1:9">
       <c r="B422" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="G422" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="H422" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="423" spans="1:9">
       <c r="C423" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="G423" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="H423" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="424" spans="1:9">
       <c r="D424" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="G424" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="H424" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="425" spans="1:9">
       <c r="D425" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="G425" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="H425" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="426" spans="1:9">
       <c r="D426" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="G426" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="H426" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="427" spans="1:9">
       <c r="D427" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="G427" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="H427" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="428" spans="1:9">
       <c r="D428" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="G428" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="H428" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="429" spans="1:9">
       <c r="E429" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="G429" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="H429" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="430" spans="1:9">
       <c r="E430" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="G430" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="H430" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="431" spans="1:9">
       <c r="E431" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="G431" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="H431" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="432" spans="1:9">
       <c r="E432" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="G432" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="H432" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="433" spans="1:9">
       <c r="E433" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="G433" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="H433" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="434" spans="1:9">
       <c r="E434" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="G434" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="H434" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="435" spans="1:9">
       <c r="D435" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="G435" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="H435" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="436" spans="1:9">
       <c r="D436" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="G436" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="H436" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="437" spans="1:9">
       <c r="E437" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="G437" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="H437" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="438" spans="1:9">
       <c r="E438" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="G438" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="H438" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="439" spans="1:9">
       <c r="D439" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="G439" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="H439" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="440" spans="1:9">
       <c r="E440" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="G440" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="H440" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="441" spans="1:9">
       <c r="E441" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="G441" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="H441" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="442" spans="1:9">
       <c r="E442" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="G442" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="H442" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="443" spans="1:9">
       <c r="D443" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="G443" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="H443" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="444" spans="1:9">
       <c r="D444" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="G444" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="H444" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="445" spans="1:9">
       <c r="D445" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="G445" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="H445" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="446" spans="1:9">
       <c r="D446" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="G446" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="H446" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="447" spans="1:9">
       <c r="D447" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="G447" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="H447" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="448" spans="1:9">
       <c r="C448" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="G448" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="H448" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="449" spans="1:9">
       <c r="D449" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="G449" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="H449" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="450" spans="1:9">
       <c r="E450" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="G450" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="H450" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="451" spans="1:9">
       <c r="E451" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="G451" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="H451" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="452" spans="1:9">
       <c r="E452" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="G452" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="H452" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="453" spans="1:9">
       <c r="D453" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="G453" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="H453" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="454" spans="1:9">
       <c r="D454" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="G454" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="H454" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="455" spans="1:9">
       <c r="D455" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="G455" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="H455" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="456" spans="1:9">
       <c r="D456" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="G456" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="H456" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="457" spans="1:9">
       <c r="D457" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="G457" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="H457" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="458" spans="1:9">
       <c r="C458" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="G458" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="H458" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="459" spans="1:9">
       <c r="D459" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="G459" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="H459" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="460" spans="1:9">
       <c r="D460" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="F460" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="G460" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="H460" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="461" spans="1:9">
       <c r="D461" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="G461" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="H461" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="462" spans="1:9">
       <c r="D462" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="G462" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="H462" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="463" spans="1:9">
       <c r="C463" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="G463" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="H463" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="464" spans="1:9">
       <c r="D464" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="G464" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="H464" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="465" spans="1:9">
       <c r="E465" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="G465" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="H465" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="466" spans="1:9">
       <c r="E466" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="G466" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="H466" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="467" spans="1:9">
       <c r="E467" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="G467" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="H467" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="468" spans="1:9">
       <c r="E468" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="G468" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="H468" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="469" spans="1:9">
       <c r="E469" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="G469" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="H469" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="470" spans="1:9">
       <c r="E470" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="G470" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="H470" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="471" spans="1:9">
       <c r="E471" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="G471" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="H471" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="472" spans="1:9">
       <c r="E472" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="G472" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="H472" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="473" spans="1:9">
       <c r="D473" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="G473" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="H473" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="474" spans="1:9">
       <c r="D474" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="G474" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="H474" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="475" spans="1:9">
       <c r="D475" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="G475" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="H475" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="476" spans="1:9">
       <c r="E476" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="G476" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="H476" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="477" spans="1:9">
       <c r="E477" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="G477" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="H477" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="478" spans="1:9">
       <c r="E478" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="G478" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="H478" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="479" spans="1:9">
       <c r="E479" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="G479" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="H479" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="480" spans="1:9">
       <c r="E480" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="G480" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="H480" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="481" spans="1:9">
       <c r="E481" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="G481" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="H481" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="482" spans="1:9">
       <c r="D482" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="G482" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="H482" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="483" spans="1:9">
       <c r="E483" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="G483" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="H483" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="484" spans="1:9">
       <c r="E484" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="G484" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="H484" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="485" spans="1:9">
       <c r="D485" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="G485" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="H485" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="486" spans="1:9">
       <c r="D486" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="G486" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="H486" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="487" spans="1:9">
       <c r="C487" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="G487" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="H487" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="488" spans="1:9">
       <c r="D488" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="G488" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="H488" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="489" spans="1:9">
       <c r="D489" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="G489" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="H489" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="490" spans="1:9">
       <c r="D490" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="G490" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="H490" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="491" spans="1:9">
       <c r="E491" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="G491" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
       <c r="H491" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="492" spans="1:9">
       <c r="E492" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="G492" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="H492" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="493" spans="1:9">
       <c r="E493" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="G493" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="H493" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="494" spans="1:9">
       <c r="E494" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="G494" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
       <c r="H494" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="495" spans="1:9">
       <c r="E495" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="G495" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="H495" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="496" spans="1:9">
       <c r="D496" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
       <c r="F496" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="G496" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="H496" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="497" spans="1:9">
       <c r="E497" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="G497" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="H497" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="498" spans="1:9">
       <c r="E498" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="G498" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="H498" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="499" spans="1:9">
       <c r="E499" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="G499" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="H499" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="500" spans="1:9">
       <c r="E500" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="G500" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="H500" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="501" spans="1:9">
       <c r="D501" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="F501" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="G501" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="H501" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="502" spans="1:9">
       <c r="E502" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="G502" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="H502" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="503" spans="1:9">
       <c r="E503" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="G503" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="H503" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="504" spans="1:9">
       <c r="E504" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="G504" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="H504" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="505" spans="1:9">
       <c r="E505" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="G505" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="H505" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="506" spans="1:9">
       <c r="E506" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="G506" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="H506" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="507" spans="1:9">
       <c r="E507" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="G507" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="H507" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="508" spans="1:9">
       <c r="E508" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="G508" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="H508" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="509" spans="1:9">
       <c r="D509" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="F509" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="G509" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="H509" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="510" spans="1:9">
       <c r="E510" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="G510" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="H510" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="511" spans="1:9">
       <c r="E511" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="G511" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="H511" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="512" spans="1:9">
       <c r="E512" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="G512" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="H512" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="513" spans="1:9">
       <c r="E513" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="G513" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="H513" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="514" spans="1:9">
       <c r="E514" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="G514" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="H514" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="515" spans="1:9">
       <c r="E515" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="G515" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="H515" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="516" spans="1:9">
       <c r="E516" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="G516" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="H516" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="517" spans="1:9">
       <c r="D517" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="G517" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="H517" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="518" spans="1:9">
       <c r="D518" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="G518" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="H518" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="519" spans="1:9">
       <c r="E519" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="G519" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="H519" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="520" spans="1:9">
       <c r="E520" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="G520" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="H520" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="521" spans="1:9">
       <c r="E521" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="G521" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="H521" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="522" spans="1:9">
       <c r="C522" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="G522" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="H522" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="523" spans="1:9">
       <c r="D523" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="F523" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="G523" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="H523" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="524" spans="1:9">
       <c r="E524" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="G524" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="H524" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="525" spans="1:9">
       <c r="E525" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="G525" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="H525" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="526" spans="1:9">
       <c r="E526" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="G526" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="H526" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="527" spans="1:9">
       <c r="E527" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="G527" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="H527" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="528" spans="1:9">
       <c r="D528" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="F528" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="G528" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="H528" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="529" spans="1:9">
       <c r="E529" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="G529" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="H529" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="530" spans="1:9">
       <c r="E530" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="G530" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="H530" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="531" spans="1:9">
       <c r="E531" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="G531" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="H531" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="532" spans="1:9">
       <c r="E532" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="G532" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="H532" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="533" spans="1:9">
       <c r="E533" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="G533" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="H533" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="534" spans="1:9">
       <c r="E534" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="G534" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="H534" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="535" spans="1:9">
       <c r="D535" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="G535" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="H535" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="536" spans="1:9">
       <c r="E536" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="F536" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="G536" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="H536" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="537" spans="1:9">
       <c r="E537" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="G537" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="H537" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="538" spans="1:9">
       <c r="E538" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="G538" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="H538" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="539" spans="1:9">
       <c r="E539" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="G539" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="H539" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="540" spans="1:9">
       <c r="E540" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="G540" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="H540" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="541" spans="1:9">
       <c r="E541" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="G541" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="H541" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="542" spans="1:9">
       <c r="D542" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="G542" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="H542" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="543" spans="1:9">
       <c r="E543" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="G543" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="H543" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="544" spans="1:9">
       <c r="E544" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="G544" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="H544" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="545" spans="1:9">
       <c r="E545" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="G545" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="H545" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="546" spans="1:9">
       <c r="E546" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="G546" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="H546" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="547" spans="1:9">
       <c r="E547" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="G547" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="H547" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="548" spans="1:9">
       <c r="D548" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="G548" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="H548" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="549" spans="1:9">
       <c r="E549" t="s">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="G549" t="s">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="H549" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="550" spans="1:9">
       <c r="E550" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="G550" t="s">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="H550" t="s">
-        <v>1666</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="551" spans="1:9">
       <c r="E551" t="s">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="G551" t="s">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="H551" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="552" spans="1:9">
       <c r="A552" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="F552" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="G552" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="H552" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="I552" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="553" spans="1:9">
       <c r="B553" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="F553" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="G553" t="s">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="H553" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="I553" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="554" spans="1:9">
       <c r="C554" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="G554" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="H554" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="I554" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="555" spans="1:9">
       <c r="C555" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="G555" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="556" spans="1:9">
       <c r="B556" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="F556" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="G556" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="557" spans="1:9">
       <c r="C557" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="G557" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="558" spans="1:9">
       <c r="C558" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="G558" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="559" spans="1:9">
       <c r="B559" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="F559" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="G559" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="560" spans="1:9">
       <c r="C560" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="G560" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="561" spans="1:9">
       <c r="C561" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="G561" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="562" spans="1:9">
       <c r="B562" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="F562" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="G562" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="563" spans="1:9">
       <c r="C563" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="G563" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="564" spans="1:9">
       <c r="C564" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="G564" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="565" spans="1:9">
       <c r="C565" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="G565" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="566" spans="1:9">
       <c r="C566" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="G566" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="567" spans="1:9">
       <c r="C567" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="G567" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="568" spans="1:9">
       <c r="C568" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="G568" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="569" spans="1:9">
       <c r="D569" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="F569" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="G569" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="570" spans="1:9">
       <c r="D570" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="F570" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="G570" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="571" spans="1:9">
       <c r="D571" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="F571" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="G571" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="572" spans="1:9">
       <c r="D572" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="F572" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="G572" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="573" spans="1:9">
       <c r="B573" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="F573" t="s">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="G573" t="s">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="H573" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="574" spans="1:9">
       <c r="C574" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="F574" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="G574" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="H574" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="575" spans="1:9">
       <c r="C575" t="s">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="F575" t="s">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="G575" t="s">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="H575" t="s">
-        <v>1737</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="576" spans="1:9">
       <c r="C576" t="s">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="G576" t="s">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="H576" t="s">
-        <v>1740</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="577" spans="1:9">
       <c r="C577" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="F577" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="G577" t="s">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="H577" t="s">
         <v>518</v>
@@ -12815,10 +12825,10 @@
     </row>
     <row r="578" spans="1:9">
       <c r="C578" t="s">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="G578" t="s">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="H578" t="s">
         <v>529</v>
@@ -12829,7 +12839,7 @@
         <v>516</v>
       </c>
       <c r="G579" t="s">
-        <v>1746</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="580" spans="1:9">
@@ -12837,133 +12847,133 @@
         <v>527</v>
       </c>
       <c r="G580" t="s">
-        <v>1747</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="581" spans="1:9">
       <c r="A581" t="s">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="F581" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="G581" t="s">
-        <v>1750</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="582" spans="1:9">
       <c r="B582" t="s">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="G582" t="s">
-        <v>1752</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="583" spans="1:9">
       <c r="C583" t="s">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="G583" t="s">
-        <v>1754</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="584" spans="1:9">
       <c r="D584" t="s">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="G584" t="s">
-        <v>1756</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="585" spans="1:9">
       <c r="E585" t="s">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="G585" t="s">
-        <v>1758</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="586" spans="1:9">
       <c r="E586" t="s">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="G586" t="s">
-        <v>1760</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="587" spans="1:9">
       <c r="E587" t="s">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="G587" t="s">
-        <v>1762</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="588" spans="1:9">
       <c r="E588" t="s">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="G588" t="s">
-        <v>1764</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="589" spans="1:9">
       <c r="D589" t="s">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="G589" t="s">
-        <v>1766</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="590" spans="1:9">
       <c r="D590" t="s">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="G590" t="s">
-        <v>1768</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="591" spans="1:9">
       <c r="D591" t="s">
-        <v>1769</v>
+        <v>1770</v>
       </c>
       <c r="F591" t="s">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="G591" t="s">
-        <v>1771</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="592" spans="1:9">
       <c r="D592" t="s">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="G592" t="s">
-        <v>1773</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="593" spans="1:9">
       <c r="D593" t="s">
-        <v>1774</v>
+        <v>1775</v>
       </c>
       <c r="G593" t="s">
-        <v>1775</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="594" spans="1:9">
       <c r="D594" t="s">
-        <v>1776</v>
+        <v>1777</v>
       </c>
       <c r="G594" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="595" spans="1:9">
       <c r="D595" t="s">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="G595" t="s">
-        <v>1779</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="596" spans="1:9">
@@ -12971,39 +12981,39 @@
         <v>527</v>
       </c>
       <c r="G596" t="s">
-        <v>1780</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="597" spans="1:9">
       <c r="E597" t="s">
-        <v>1781</v>
+        <v>1782</v>
       </c>
       <c r="G597" t="s">
-        <v>1782</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="598" spans="1:9">
       <c r="D598" t="s">
-        <v>1783</v>
+        <v>1784</v>
       </c>
       <c r="G598" t="s">
-        <v>1784</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="599" spans="1:9">
       <c r="D599" t="s">
-        <v>1785</v>
+        <v>1786</v>
       </c>
       <c r="G599" t="s">
-        <v>1786</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="600" spans="1:9">
       <c r="D600" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="G600" t="s">
-        <v>1788</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="601" spans="1:9">
@@ -13011,834 +13021,833 @@
         <v>209</v>
       </c>
       <c r="G601" t="s">
-        <v>1789</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="602" spans="1:9">
       <c r="D602" t="s">
-        <v>1790</v>
+        <v>1791</v>
       </c>
       <c r="F602" t="s">
-        <v>1791</v>
+        <v>1792</v>
       </c>
       <c r="G602" t="s">
-        <v>1792</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="603" spans="1:9">
       <c r="D603" t="s">
-        <v>1793</v>
+        <v>1794</v>
       </c>
       <c r="G603" t="s">
-        <v>1794</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="604" spans="1:9">
       <c r="D604" t="s">
-        <v>1795</v>
+        <v>1796</v>
       </c>
       <c r="G604" t="s">
-        <v>1796</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="605" spans="1:9">
       <c r="C605" t="s">
-        <v>1797</v>
+        <v>1798</v>
       </c>
       <c r="G605" t="s">
-        <v>1798</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="606" spans="1:9">
       <c r="D606" t="s">
-        <v>1799</v>
+        <v>1800</v>
       </c>
       <c r="F606" t="s">
-        <v>1800</v>
+        <v>1801</v>
       </c>
       <c r="G606" t="s">
-        <v>1801</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="607" spans="1:9">
       <c r="D607" t="s">
-        <v>1802</v>
+        <v>1803</v>
       </c>
       <c r="G607" t="s">
-        <v>1803</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="608" spans="1:9">
       <c r="D608" t="s">
-        <v>1804</v>
+        <v>1805</v>
       </c>
       <c r="G608" t="s">
-        <v>1805</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="609" spans="1:9">
       <c r="E609" t="s">
-        <v>1806</v>
+        <v>1807</v>
       </c>
       <c r="G609" t="s">
-        <v>1807</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="610" spans="1:9">
       <c r="D610" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="G610" t="s">
-        <v>1809</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="611" spans="1:9">
       <c r="D611" t="s">
-        <v>1810</v>
+        <v>1811</v>
       </c>
       <c r="G611" t="s">
-        <v>1811</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="612" spans="1:9">
       <c r="D612" t="s">
-        <v>1812</v>
+        <v>1813</v>
       </c>
       <c r="G612" t="s">
-        <v>1813</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="613" spans="1:9">
       <c r="C613" t="s">
-        <v>1814</v>
+        <v>1815</v>
       </c>
       <c r="G613" t="s">
-        <v>1815</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="614" spans="1:9">
       <c r="D614" t="s">
-        <v>1816</v>
+        <v>1817</v>
       </c>
       <c r="G614" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="615" spans="1:9">
       <c r="D615" t="s">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="G615" t="s">
-        <v>1819</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="616" spans="1:9">
       <c r="D616" t="s">
-        <v>1820</v>
+        <v>1821</v>
       </c>
       <c r="G616" t="s">
-        <v>1821</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="617" spans="1:9">
       <c r="D617" t="s">
-        <v>1822</v>
+        <v>1823</v>
       </c>
       <c r="G617" t="s">
-        <v>1823</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="618" spans="1:9">
       <c r="C618" t="s">
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="G618" t="s">
-        <v>1825</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="619" spans="1:9">
       <c r="D619" t="s">
-        <v>1826</v>
+        <v>1827</v>
       </c>
       <c r="G619" t="s">
-        <v>1827</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="620" spans="1:9">
       <c r="D620" t="s">
-        <v>1828</v>
+        <v>1829</v>
       </c>
       <c r="G620" t="s">
-        <v>1829</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="621" spans="1:9">
       <c r="D621" t="s">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="G621" t="s">
-        <v>1831</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="622" spans="1:9">
       <c r="D622" t="s">
-        <v>1832</v>
+        <v>1833</v>
       </c>
       <c r="G622" t="s">
-        <v>1833</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="623" spans="1:9">
       <c r="D623" t="s">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="G623" t="s">
-        <v>1835</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="624" spans="1:9">
       <c r="D624" t="s">
-        <v>1836</v>
+        <v>1837</v>
       </c>
       <c r="G624" t="s">
-        <v>1837</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="625" spans="1:9">
       <c r="D625" t="s">
-        <v>1838</v>
+        <v>1839</v>
       </c>
       <c r="G625" t="s">
-        <v>1839</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="626" spans="1:9">
       <c r="D626" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="G626" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="627" spans="1:9">
       <c r="D627" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="G627" t="s">
-        <v>1843</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="628" spans="1:9">
       <c r="B628" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="G628" t="s">
-        <v>1845</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="629" spans="1:9">
       <c r="C629" t="s">
-        <v>1846</v>
+        <v>1847</v>
       </c>
       <c r="G629" t="s">
-        <v>1847</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="630" spans="1:9">
       <c r="D630" t="s">
-        <v>1848</v>
+        <v>1849</v>
       </c>
       <c r="F630" t="s">
-        <v>1849</v>
+        <v>1850</v>
       </c>
       <c r="G630" t="s">
-        <v>1850</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="631" spans="1:9">
       <c r="E631" t="s">
-        <v>1851</v>
+        <v>1852</v>
       </c>
       <c r="F631" t="s">
-        <v>1852</v>
+        <v>1853</v>
       </c>
       <c r="G631" t="s">
-        <v>1853</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="632" spans="1:9">
       <c r="E632" t="s">
-        <v>1854</v>
+        <v>1855</v>
       </c>
       <c r="G632" t="s">
-        <v>1855</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="633" spans="1:9">
       <c r="E633" t="s">
-        <v>1856</v>
+        <v>1857</v>
       </c>
       <c r="F633" t="s">
-        <v>1857</v>
+        <v>1858</v>
       </c>
       <c r="G633" t="s">
-        <v>1858</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="634" spans="1:9">
       <c r="E634" t="s">
-        <v>1859</v>
+        <v>1860</v>
       </c>
       <c r="F634" t="s">
-        <v>1860</v>
+        <v>1861</v>
       </c>
       <c r="G634" t="s">
-        <v>1861</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="635" spans="1:9">
       <c r="E635" t="s">
-        <v>1862</v>
+        <v>1863</v>
       </c>
       <c r="G635" t="s">
-        <v>1863</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="636" spans="1:9">
       <c r="E636" t="s">
-        <v>1864</v>
+        <v>1865</v>
       </c>
       <c r="G636" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="637" spans="1:9">
       <c r="E637" t="s">
-        <v>1866</v>
+        <v>1867</v>
       </c>
       <c r="G637" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="638" spans="1:9">
       <c r="E638" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="G638" t="s">
-        <v>1869</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="639" spans="1:9">
       <c r="D639" t="s">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="F639" t="s">
-        <v>1871</v>
+        <v>1872</v>
       </c>
       <c r="G639" t="s">
-        <v>1872</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="640" spans="1:9">
       <c r="E640" t="s">
-        <v>1873</v>
+        <v>1874</v>
       </c>
       <c r="G640" t="s">
-        <v>1874</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="641" spans="1:9">
       <c r="E641" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="F641" t="s">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="G641" t="s">
-        <v>1877</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="642" spans="1:9">
       <c r="E642" t="s">
-        <v>1878</v>
+        <v>1879</v>
       </c>
       <c r="G642" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="643" spans="1:9">
       <c r="C643" t="s">
-        <v>1880</v>
+        <v>1881</v>
       </c>
       <c r="G643" t="s">
-        <v>1881</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="644" spans="1:9">
       <c r="D644" t="s">
-        <v>1882</v>
+        <v>1883</v>
       </c>
       <c r="F644" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="G644" t="s">
-        <v>1884</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="645" spans="1:9">
       <c r="D645" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
       <c r="G645" t="s">
-        <v>1886</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="646" spans="1:9">
       <c r="D646" t="s">
-        <v>1887</v>
+        <v>1888</v>
       </c>
       <c r="F646" t="s">
-        <v>1888</v>
+        <v>1889</v>
       </c>
       <c r="G646" t="s">
-        <v>1889</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="647" spans="1:9">
       <c r="D647" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="F647" t="s">
-        <v>1891</v>
+        <v>1892</v>
       </c>
       <c r="G647" t="s">
-        <v>1892</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="648" spans="1:9">
       <c r="D648" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="G648" t="s">
-        <v>1894</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="649" spans="1:9">
       <c r="D649" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="G649" t="s">
-        <v>1896</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="650" spans="1:9">
       <c r="D650" t="s">
-        <v>1897</v>
+        <v>1898</v>
       </c>
       <c r="G650" t="s">
-        <v>1898</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="651" spans="1:9">
       <c r="D651" t="s">
-        <v>1899</v>
+        <v>1900</v>
       </c>
       <c r="G651" t="s">
-        <v>1900</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="652" spans="1:9">
       <c r="D652" t="s">
-        <v>1901</v>
+        <v>1902</v>
       </c>
       <c r="G652" t="s">
-        <v>1902</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="653" spans="1:9">
       <c r="D653" t="s">
-        <v>1903</v>
+        <v>1904</v>
       </c>
       <c r="F653" t="s">
-        <v>1904</v>
+        <v>1905</v>
       </c>
       <c r="G653" t="s">
-        <v>1905</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="654" spans="1:9">
       <c r="B654" t="s">
-        <v>1906</v>
+        <v>1907</v>
       </c>
       <c r="F654" t="s">
-        <v>1907</v>
+        <v>1908</v>
       </c>
       <c r="G654" t="s">
-        <v>1908</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="655" spans="1:9">
       <c r="C655" t="s">
-        <v>1909</v>
+        <v>1910</v>
       </c>
       <c r="G655" t="s">
-        <v>1910</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="656" spans="1:9">
       <c r="D656" t="s">
-        <v>1911</v>
+        <v>1912</v>
       </c>
       <c r="G656" t="s">
-        <v>1912</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="657" spans="1:9">
       <c r="D657" t="s">
-        <v>1913</v>
+        <v>1914</v>
       </c>
       <c r="G657" t="s">
-        <v>1914</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="658" spans="1:9">
       <c r="C658" t="s">
-        <v>1915</v>
+        <v>1916</v>
       </c>
       <c r="G658" t="s">
-        <v>1916</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="659" spans="1:9">
       <c r="D659" t="s">
-        <v>1917</v>
+        <v>1918</v>
       </c>
       <c r="F659" t="s">
-        <v>1918</v>
+        <v>1919</v>
       </c>
       <c r="G659" t="s">
-        <v>1919</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="660" spans="1:9">
       <c r="D660" t="s">
-        <v>1920</v>
+        <v>1921</v>
       </c>
       <c r="G660" t="s">
-        <v>1921</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="661" spans="1:9">
       <c r="D661" t="s">
-        <v>1922</v>
+        <v>1923</v>
       </c>
       <c r="G661" t="s">
-        <v>1923</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="662" spans="1:9">
       <c r="D662" t="s">
-        <v>1913</v>
+        <v>1914</v>
       </c>
       <c r="G662" t="s">
-        <v>1924</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="663" spans="1:9">
       <c r="D663" t="s">
-        <v>1925</v>
+        <v>1926</v>
       </c>
       <c r="G663" t="s">
-        <v>1926</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="664" spans="1:9">
       <c r="D664" t="s">
-        <v>1927</v>
+        <v>1928</v>
       </c>
       <c r="G664" t="s">
-        <v>1928</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="665" spans="1:9">
       <c r="D665" t="s">
-        <v>1812</v>
+        <v>1813</v>
       </c>
       <c r="G665" t="s">
-        <v>1929</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="666" spans="1:9">
       <c r="C666" t="s">
-        <v>1930</v>
+        <v>1931</v>
       </c>
       <c r="G666" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="667" spans="1:9">
       <c r="D667" t="s">
-        <v>1932</v>
+        <v>1933</v>
       </c>
       <c r="G667" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="668" spans="1:9">
       <c r="D668" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="G668" t="s">
-        <v>1935</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="669" spans="1:9">
       <c r="D669" t="s">
-        <v>1936</v>
+        <v>1937</v>
       </c>
       <c r="G669" t="s">
-        <v>1937</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="670" spans="1:9">
       <c r="D670" t="s">
-        <v>1938</v>
+        <v>1939</v>
       </c>
       <c r="F670" t="s">
-        <v>1939</v>
+        <v>1940</v>
       </c>
       <c r="G670" t="s">
-        <v>1940</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="671" spans="1:9">
       <c r="D671" t="s">
-        <v>1941</v>
+        <v>1942</v>
       </c>
       <c r="G671" t="s">
-        <v>1942</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="672" spans="1:9">
       <c r="D672" t="s">
-        <v>1943</v>
+        <v>1944</v>
       </c>
       <c r="G672" t="s">
-        <v>1944</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="673" spans="1:9">
       <c r="D673" t="s">
-        <v>1945</v>
+        <v>1946</v>
       </c>
       <c r="G673" t="s">
-        <v>1946</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="674" spans="1:9">
       <c r="B674" t="s">
-        <v>1947</v>
+        <v>1948</v>
       </c>
       <c r="G674" t="s">
-        <v>1948</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="675" spans="1:9">
       <c r="C675" t="s">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="G675" t="s">
-        <v>1950</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="676" spans="1:9">
       <c r="D676" t="s">
-        <v>1951</v>
+        <v>1952</v>
       </c>
       <c r="G676" t="s">
-        <v>1952</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="677" spans="1:9">
       <c r="C677" t="s">
-        <v>1953</v>
+        <v>1954</v>
       </c>
       <c r="G677" t="s">
-        <v>1954</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="678" spans="1:9">
       <c r="D678" t="s">
-        <v>1955</v>
+        <v>1956</v>
       </c>
       <c r="G678" t="s">
-        <v>1956</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="679" spans="1:9">
       <c r="D679" t="s">
-        <v>1957</v>
+        <v>1958</v>
       </c>
       <c r="G679" t="s">
-        <v>1958</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="680" spans="1:9">
       <c r="D680" t="s">
-        <v>1959</v>
+        <v>1960</v>
       </c>
       <c r="G680" t="s">
-        <v>1960</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="681" spans="1:9">
       <c r="D681" t="s">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="F681" t="s">
-        <v>1962</v>
+        <v>1963</v>
       </c>
       <c r="G681" t="s">
-        <v>1963</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="682" spans="1:9">
       <c r="C682" t="s">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="G682" t="s">
-        <v>1965</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="683" spans="1:9">
       <c r="D683" t="s">
-        <v>1966</v>
+        <v>1967</v>
       </c>
       <c r="G683" t="s">
-        <v>1967</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="684" spans="1:9">
       <c r="E684" t="s">
-        <v>1968</v>
+        <v>1969</v>
       </c>
       <c r="G684" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="685" spans="1:9">
       <c r="E685" t="s">
-        <v>1970</v>
+        <v>1971</v>
       </c>
       <c r="G685" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="686" spans="1:9">
       <c r="D686" t="s">
-        <v>1972</v>
+        <v>1973</v>
       </c>
       <c r="G686" t="s">
-        <v>1973</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="687" spans="1:9">
       <c r="E687" t="s">
-        <v>1974</v>
+        <v>1975</v>
       </c>
       <c r="G687" t="s">
-        <v>1975</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="688" spans="1:9">
       <c r="A688" t="s">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="F688" t="s">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="G688" t="s">
-        <v>1978</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="689" spans="1:9">
       <c r="B689" t="s">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="F689" t="s">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="G689" t="s">
-        <v>1981</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="690" spans="1:9">
       <c r="B690" t="s">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="F690" t="s">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="G690" t="s">
-        <v>1984</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="691" spans="1:9">
       <c r="B691" t="s">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="F691" t="s">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="G691" t="s">
-        <v>1987</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="692" spans="1:9">
       <c r="B692" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="G692" t="s">
-        <v>1989</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="693" spans="1:9">
       <c r="B693" t="s">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="F693" t="s">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="G693" t="s">
-        <v>1992</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="694" spans="1:9">
       <c r="C694" t="s">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="G694" t="s">
-        <v>1994</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="695" spans="1:9">
       <c r="C695" t="s">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="G695" t="s">
-        <v>1996</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="696" spans="1:9">
       <c r="C696" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="G696" t="s">
-        <v>1998</v>
+        <v>1999</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
@@ -13850,5 +13859,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>